<commit_message>
From bp to pp
</commit_message>
<xml_diff>
--- a/CIVICS_Ghana/Water_gap.xlsx
+++ b/CIVICS_Ghana/Water_gap.xlsx
@@ -1,32 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\FEEM\CIVICS_Ghana\Simplified\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\CIVICS\CIVICS_Ghana\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E43E2A-D62D-442F-A4B3-DA4B12AB9DA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11508" windowHeight="8508" activeTab="1"/>
+    <workbookView xWindow="-38520" yWindow="-5445" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="65">
   <si>
     <t>Ashanti</t>
   </si>
@@ -235,15 +245,27 @@
   <si>
     <t>Blue Water (million cubic meters)</t>
   </si>
+  <si>
+    <t>ha/farmer</t>
+  </si>
+  <si>
+    <t>kWh/farmer/month</t>
+  </si>
+  <si>
+    <t>Data for crop area</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,6 +282,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -542,10 +571,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -594,6 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -624,9 +655,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -904,109 +940,110 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BG29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BH29"/>
   <sheetViews>
-    <sheetView zoomScale="88" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AT1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AZ21" sqref="AZ21"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="AZ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.26171875" customWidth="1"/>
-    <col min="2" max="2" width="47.734375" customWidth="1"/>
-    <col min="3" max="3" width="38.62890625" customWidth="1"/>
-    <col min="17" max="17" width="29.5234375" customWidth="1"/>
-    <col min="18" max="18" width="19.83984375" customWidth="1"/>
-    <col min="19" max="19" width="19.3125" customWidth="1"/>
-    <col min="21" max="21" width="20.05078125" customWidth="1"/>
-    <col min="26" max="26" width="25.7890625" customWidth="1"/>
-    <col min="39" max="39" width="22.7890625" customWidth="1"/>
-    <col min="46" max="46" width="22.47265625" customWidth="1"/>
-    <col min="47" max="47" width="17.3125" customWidth="1"/>
-    <col min="48" max="48" width="11.26171875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.47265625" customWidth="1"/>
-    <col min="52" max="52" width="32.62890625" customWidth="1"/>
-    <col min="58" max="58" width="18.05078125" customWidth="1"/>
+    <col min="1" max="1" width="43.21875" customWidth="1"/>
+    <col min="2" max="2" width="47.77734375" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="17" max="17" width="29.5546875" customWidth="1"/>
+    <col min="18" max="18" width="19.88671875" customWidth="1"/>
+    <col min="19" max="19" width="19.33203125" customWidth="1"/>
+    <col min="21" max="21" width="20" customWidth="1"/>
+    <col min="26" max="26" width="25.77734375" customWidth="1"/>
+    <col min="39" max="39" width="22.77734375" customWidth="1"/>
+    <col min="46" max="46" width="22.44140625" customWidth="1"/>
+    <col min="47" max="47" width="17.33203125" customWidth="1"/>
+    <col min="48" max="48" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.44140625" customWidth="1"/>
+    <col min="52" max="52" width="9.77734375" customWidth="1"/>
+    <col min="53" max="53" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="48" t="s">
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="49"/>
-      <c r="U1" s="49"/>
-      <c r="V1" s="49"/>
-      <c r="W1" s="49"/>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="48" t="s">
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="AB1" s="49"/>
-      <c r="AC1" s="49"/>
-      <c r="AD1" s="49"/>
-      <c r="AE1" s="49"/>
-      <c r="AF1" s="49"/>
-      <c r="AG1" s="49"/>
-      <c r="AH1" s="49"/>
-      <c r="AI1" s="49"/>
-      <c r="AJ1" s="49"/>
-      <c r="AK1" s="49"/>
-      <c r="AL1" s="49"/>
-      <c r="AM1" s="51" t="s">
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50"/>
+      <c r="AE1" s="50"/>
+      <c r="AF1" s="50"/>
+      <c r="AG1" s="50"/>
+      <c r="AH1" s="50"/>
+      <c r="AI1" s="50"/>
+      <c r="AJ1" s="50"/>
+      <c r="AK1" s="50"/>
+      <c r="AL1" s="50"/>
+      <c r="AM1" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="AN1" s="52"/>
-      <c r="AO1" s="52"/>
-      <c r="AP1" s="52"/>
-      <c r="AQ1" s="52"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="45" t="s">
+      <c r="AN1" s="53"/>
+      <c r="AO1" s="53"/>
+      <c r="AP1" s="53"/>
+      <c r="AQ1" s="53"/>
+      <c r="AR1" s="54"/>
+      <c r="AS1" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
-      <c r="AW1" s="46"/>
-      <c r="AX1" s="47"/>
-      <c r="AY1" s="45" t="s">
+      <c r="AT1" s="47"/>
+      <c r="AU1" s="47"/>
+      <c r="AV1" s="47"/>
+      <c r="AW1" s="47"/>
+      <c r="AX1" s="48"/>
+      <c r="AY1" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="AZ1" s="46"/>
-      <c r="BA1" s="46"/>
-      <c r="BB1" s="46"/>
-      <c r="BC1" s="46"/>
-      <c r="BD1" s="47"/>
+      <c r="AZ1" s="47"/>
+      <c r="BA1" s="47"/>
+      <c r="BB1" s="47"/>
+      <c r="BC1" s="47"/>
+      <c r="BD1" s="48"/>
     </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
@@ -1176,7 +1213,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1336,7 +1373,7 @@
         <v>14704.983549013181</v>
       </c>
       <c r="BD3" s="28"/>
-      <c r="BF3" s="31">
+      <c r="BF3" s="55">
         <f>SUM(BA3:BB12)*13*30*0.35/10^6</f>
         <v>27.314317857447342</v>
       </c>
@@ -1344,7 +1381,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1504,7 +1541,7 @@
       <c r="BD4" s="28"/>
       <c r="BF4" s="31"/>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1662,11 +1699,11 @@
         <v>10125.218355999794</v>
       </c>
       <c r="BD5" s="28"/>
-      <c r="BF5" s="54">
+      <c r="BF5" s="44">
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1825,7 +1862,7 @@
       </c>
       <c r="BD6" s="28"/>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -1994,8 +2031,18 @@
         <v>496.33931509942323</v>
       </c>
       <c r="BD7" s="28"/>
+      <c r="BF7">
+        <v>2011180</v>
+      </c>
+      <c r="BG7" s="57">
+        <f>BA13/BF7</f>
+        <v>6.4967939168439764E-2</v>
+      </c>
+      <c r="BH7" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -2165,8 +2212,19 @@
         <v>5128.7140022762569</v>
       </c>
       <c r="BD8" s="28"/>
+      <c r="BF8">
+        <f>SUM(B3:B12)</f>
+        <v>1022463.1</v>
+      </c>
+      <c r="BG8" s="58">
+        <f>BF8/BF7</f>
+        <v>0.50838965184617979</v>
+      </c>
+      <c r="BH8" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -2324,8 +2382,14 @@
         <v>3351.6312696041732</v>
       </c>
       <c r="BD9" s="28"/>
+      <c r="BG9" s="59">
+        <v>2017</v>
+      </c>
+      <c r="BH9" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -2484,7 +2548,7 @@
       </c>
       <c r="BD10" s="28"/>
     </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -2655,7 +2719,7 @@
       </c>
       <c r="BD11" s="28"/>
     </row>
-    <row r="12" spans="1:59" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:60" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
@@ -2826,7 +2890,17 @@
       </c>
       <c r="BD12" s="30"/>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:60" x14ac:dyDescent="0.3">
+      <c r="BA13" s="56">
+        <f>SUM(BA3:BA12)</f>
+        <v>130662.21989678268</v>
+      </c>
+      <c r="BB13">
+        <f>SUM(BB3:BB12)</f>
+        <v>69442.672831769276</v>
+      </c>
+    </row>
+    <row r="15" spans="1:60" x14ac:dyDescent="0.3">
       <c r="Q15" s="17" t="s">
         <v>33</v>
       </c>
@@ -2840,10 +2914,10 @@
         <v>0.3</v>
       </c>
       <c r="U15" s="17"/>
-      <c r="AT15" s="44" t="s">
+      <c r="AT15" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="AU15" s="44"/>
+      <c r="AU15" s="45"/>
       <c r="AW15" s="17" t="s">
         <v>53</v>
       </c>
@@ -2851,7 +2925,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:60" x14ac:dyDescent="0.3">
       <c r="Q16" s="18" t="s">
         <v>36</v>
       </c>
@@ -2883,7 +2957,7 @@
         <v>6159.4675018914268</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.3">
       <c r="Q17" s="17" t="s">
         <v>37</v>
       </c>
@@ -2908,7 +2982,7 @@
         <v>10039.770634125114</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AT18" s="41">
         <v>121488.5567414461</v>
       </c>
@@ -2920,7 +2994,7 @@
         <v>3037.2139185361525</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2941,7 +3015,7 @@
         <v>8804.7312721331891</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -2969,7 +3043,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -2984,7 +3058,7 @@
         <v>7992.0218649505387</v>
       </c>
     </row>
-    <row r="22" spans="1:53" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -2999,7 +3073,7 @@
         <v>4763.3191881404609</v>
       </c>
     </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AT23" s="41">
         <v>196794.20185537045</v>
       </c>
@@ -3011,7 +3085,7 @@
         <v>4919.8550463842612</v>
       </c>
     </row>
-    <row r="24" spans="1:53" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AT24" s="41">
         <v>115717.96460825529</v>
       </c>
@@ -3023,7 +3097,7 @@
         <v>2892.9491152063824</v>
       </c>
     </row>
-    <row r="25" spans="1:53" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AT25" s="41">
         <v>45625.255686094257</v>
       </c>
@@ -3035,17 +3109,17 @@
         <v>1140.6313921523565</v>
       </c>
     </row>
-    <row r="26" spans="1:53" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:53" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:53" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AV29" s="43" t="s">
         <v>50</v>
       </c>
@@ -3072,21 +3146,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="12.734375" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>56</v>
       </c>
@@ -3097,7 +3171,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>59</v>
       </c>
@@ -3106,7 +3180,7 @@
         <v>27.314317857447342</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="43" t="s">
         <v>60</v>
       </c>
@@ -3115,7 +3189,7 @@
         <v>449.5259858834267</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="43" t="s">
         <v>54</v>
       </c>
@@ -3124,7 +3198,7 @@
         <v>0.26845637583892612</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="43" t="s">
         <v>61</v>
       </c>
@@ -3139,12 +3213,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>